<commit_message>
adding inline code, table and reference, writing results and introduction
</commit_message>
<xml_diff>
--- a/Data/MLB.xlsx
+++ b/Data/MLB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woock/Documents/edld_610_finalproject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780C1312-FE6A-CE49-9E3E-D4294A523578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF823ECE-826B-6149-8570-433262C4B48D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" xr2:uid="{18CDC568-5170-FC4C-B874-E6D6AB372BFE}"/>
   </bookViews>
@@ -939,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B42A43-8E5D-534F-A043-61864287759A}">
   <dimension ref="A1:W529"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
-      <selection activeCell="G385" sqref="G385"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
writing results and adding titles for table and inline
</commit_message>
<xml_diff>
--- a/Data/MLB.xlsx
+++ b/Data/MLB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woock/Documents/edld_610_finalproject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF823ECE-826B-6149-8570-433262C4B48D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12989BA-3F04-9A44-BED7-2AC053D403C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" xr2:uid="{18CDC568-5170-FC4C-B874-E6D6AB372BFE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{18CDC568-5170-FC4C-B874-E6D6AB372BFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -620,6 +620,7 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -939,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B42A43-8E5D-534F-A043-61864287759A}">
   <dimension ref="A1:W529"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2432,7 +2433,7 @@
       <c r="G41">
         <v>34077</v>
       </c>
-      <c r="H41" s="19">
+      <c r="H41" s="35">
         <v>1921844</v>
       </c>
       <c r="I41">

</xml_diff>